<commit_message>
Initial 3217xpro_QT7 project from v25 platform
</commit_message>
<xml_diff>
--- a/doc/wire connection.xlsx
+++ b/doc/wire connection.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\a41450\atmel studio\ATtiny3217-1Finger-Low_Power-Project-MPT2\ATtiny3217-1Finger-Low_Power-Project-MPT2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6A0B09-A263-4416-B3CE-949C037AF5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09F8302-5721-4B1C-BD9F-7E0BB5B2E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9144" yWindow="1872" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="qt7" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>D21 Xpro</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +110,142 @@
   </si>
   <si>
     <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLD3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLD1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLD2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QT7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -116,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +289,30 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +340,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -220,23 +397,47 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -534,16 +735,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -562,70 +763,70 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -636,4 +837,244 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90B008-77F3-40F0-9120-C6AB97389858}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="10">
+        <v>8</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>11</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="10">
+        <v>12</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="10">
+        <v>14</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="10">
+        <v>16</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="10">
+        <v>18</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="10">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
firmware 1.3: build t15/t9 call back for lighting LEDs
</commit_message>
<xml_diff>
--- a/doc/wire connection.xlsx
+++ b/doc/wire connection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\a41450\atmel studio\ATtiny3217-1Finger-Low_Power-Project-MPT2\ATtiny3217-1Finger-Low_Power-Project-MPT2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09F8302-5721-4B1C-BD9F-7E0BB5B2E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F02E4-0F8E-466A-BB8C-E6CC8C2E13CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9144" yWindow="1872" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1080" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>D21 Xpro</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,6 +246,46 @@
   </si>
   <si>
     <t>Pin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slider LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>btn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -389,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -415,6 +455,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,6 +479,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,10 +888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90B008-77F3-40F0-9120-C6AB97389858}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -852,225 +899,283 @@
     <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="11">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
+    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
         <v>3</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="11">
         <v>4</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <v>6</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
         <v>7</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="11">
         <v>8</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
         <v>9</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>10</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
         <v>11</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="11">
         <v>12</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
         <v>13</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <v>14</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
         <v>15</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="11">
         <v>16</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>17</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>18</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>19</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>20</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
QT8 Platform V25 build 1.6: <1> T111 controllable with parameters <2> add `WK_RSV_NEG_BREACH` in T126 wakeup message <3> add touch_non_ptc_pin_config() at touch_init() for non PTC pin initialize <4> #define DEF_TOUCH_MEASUREMENT_OVERFLOW_FORCE_DONE 200
</commit_message>
<xml_diff>
--- a/doc/wire connection.xlsx
+++ b/doc/wire connection.xlsx
@@ -8,25 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\a41450\atmel studio\ATtiny3217-1Finger-Low_Power-Project-MPT2\ATtiny3217-1Finger-Low_Power-Project-MPT2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F02E4-0F8E-466A-BB8C-E6CC8C2E13CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D97469-FFE6-4CFC-A6FC-A69FBC029719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1080" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="I2C" sheetId="1" r:id="rId1"/>
     <sheet name="qt7" sheetId="2" r:id="rId2"/>
+    <sheet name="qt8" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
   <si>
     <t>D21 Xpro</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -286,6 +296,118 @@
   </si>
   <si>
     <t>a1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QT8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y5~9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y0~4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue that it control LED0 in 3217Xpro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PB4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PC0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Mutual cap scanning, PC0 config as Low output; For Selfcap scanning PC0 config as DS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -293,7 +415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,8 +473,29 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +544,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -429,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -452,9 +601,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,6 +632,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,7 +978,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -824,7 +992,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -890,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90B008-77F3-40F0-9120-C6AB97389858}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -900,282 +1068,574 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>3</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>4</v>
       </c>
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="10">
+        <v>8</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>11</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="10">
+        <v>12</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="10">
+        <v>14</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="10">
+        <v>16</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="11">
+        <v>18</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BE74D1-0EE0-401F-BC3B-99FCD9A9FF68}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="21">
+        <v>4</v>
+      </c>
       <c r="E3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
         <v>5</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="21">
         <v>6</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="E4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>7</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="21">
         <v>8</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>9</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="21">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>11</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="21">
         <v>12</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <v>13</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="21">
         <v>14</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>15</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="21">
         <v>16</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
         <v>17</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="19">
         <v>18</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="E10" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>19</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>20</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
3217Xpro Platform v25 build 16: <1>T111 controllable with parameters <2>add `WK_RSV_NEG_BREACH` in T126 wakeup message <3> add touch_non_ptc_pin_config() at touch_init() for non PTC pin initialize <4> #define DEF_TOUCH_MEASUREMENT_OVERFLOW_FORCE_DONE 200 <5> LED callback
</commit_message>
<xml_diff>
--- a/doc/wire connection.xlsx
+++ b/doc/wire connection.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\a41450\atmel studio\ATtiny3217-1Finger-Low_Power-Project-MPT2\ATtiny3217-1Finger-Low_Power-Project-MPT2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6A0B09-A263-4416-B3CE-949C037AF5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D97469-FFE6-4CFC-A6FC-A69FBC029719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="I2C" sheetId="1" r:id="rId1"/>
+    <sheet name="qt7" sheetId="2" r:id="rId2"/>
+    <sheet name="qt8" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
   <si>
     <t>D21 Xpro</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +120,294 @@
   </si>
   <si>
     <t>INT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLD3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLD1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTN1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLD2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QT7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slider LED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>btn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QT8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y5~9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y0~4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue that it control LED0 in 3217Xpro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PB4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PC0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Mutual cap scanning, PC0 config as Low output; For Selfcap scanning PC0 config as DS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -116,7 +415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,8 +451,51 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +523,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -220,24 +586,74 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -534,16 +950,16 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -562,70 +978,70 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -636,4 +1052,594 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90B008-77F3-40F0-9120-C6AB97389858}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>3</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="10">
+        <v>8</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>11</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="10">
+        <v>12</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="10">
+        <v>14</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="10">
+        <v>16</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="11">
+        <v>18</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BE74D1-0EE0-401F-BC3B-99FCD9A9FF68}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="21">
+        <v>4</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="21">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="21">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>9</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="21">
+        <v>10</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>11</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="21">
+        <v>12</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="21">
+        <v>14</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="21">
+        <v>16</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="19">
+        <v>18</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
QT7 Platform v25 build 16: <1> T111 controllable with parameters <2> add `WK_RSV_NEG_BREACH` in T126 wakeup message <3> add touch_non_ptc_pin_config() at touch_init() for non PTC pin initialize <4> #define DEF_TOUCH_MEASUREMENT_OVERFLOW_FORCE_DONE 200 <5> add LED0 callback when button touched
</commit_message>
<xml_diff>
--- a/doc/wire connection.xlsx
+++ b/doc/wire connection.xlsx
@@ -8,25 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\a41450\atmel studio\ATtiny3217-1Finger-Low_Power-Project-MPT2\ATtiny3217-1Finger-Low_Power-Project-MPT2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F02E4-0F8E-466A-BB8C-E6CC8C2E13CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C56F232-3096-48EC-8E40-4EB79B6C6121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1080" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="I2C" sheetId="1" r:id="rId1"/>
     <sheet name="qt7" sheetId="2" r:id="rId2"/>
+    <sheet name="qt8" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
   <si>
     <t>D21 Xpro</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -286,6 +296,122 @@
   </si>
   <si>
     <t>a1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QT8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y5~9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y0~4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue that it control LED0 in 3217Xpro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PB4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>PC0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For Mutual cap scanning, PC0 config as Low output; For Selfcap scanning PC0 config as DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue with PA1/PA2 used as IRQ/I2C communication instead of LED control</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -293,7 +419,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,8 +477,36 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +555,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -429,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -452,9 +612,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -485,6 +642,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,7 +992,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="26" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -824,7 +1006,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
@@ -888,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90B008-77F3-40F0-9120-C6AB97389858}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -899,283 +1081,578 @@
     <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>3</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>4</v>
       </c>
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="10">
+        <v>8</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>11</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="10">
+        <v>12</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="10">
+        <v>14</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>15</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="10">
+        <v>16</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>17</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="11">
+        <v>18</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11">
+        <v>20</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BE74D1-0EE0-401F-BC3B-99FCD9A9FF68}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="21">
+        <v>4</v>
+      </c>
       <c r="E3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
         <v>5</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="21">
         <v>6</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="E4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <v>7</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="21">
         <v>8</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+    <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <v>9</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="21">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+    <row r="7" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
         <v>11</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="21">
         <v>12</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+    <row r="8" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <v>13</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="21">
         <v>14</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+    <row r="9" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>15</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="21">
         <v>16</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
         <v>17</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="19">
         <v>18</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="E10" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>19</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>20</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>